<commit_message>
Updated graphs for dilution curves
</commit_message>
<xml_diff>
--- a/experimental_data/dilution_indicator/Dilution_indicator_data.xlsx
+++ b/experimental_data/dilution_indicator/Dilution_indicator_data.xlsx
@@ -79,10 +79,10 @@
     <t>Galactose</t>
   </si>
   <si>
-    <t>B: galactose 315mg/100ml | glucose 103 mg/100ml</t>
+    <t>B: galactose 225mg/100ml | glucose 103 mg/100ml</t>
   </si>
   <si>
-    <t>C: galactose 225mg/100ml | glucose 103 mg/100ml</t>
+    <t>C: galactose 315mg/100ml | glucose 118 mg/100ml</t>
   </si>
   <si>
     <t>condition</t>
@@ -403,7 +403,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -712,11 +712,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="43028982"/>
-        <c:axId val="47518773"/>
+        <c:axId val="98521956"/>
+        <c:axId val="14802157"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43028982"/>
+        <c:axId val="98521956"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -758,12 +758,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47518773"/>
+        <c:crossAx val="14802157"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47518773"/>
+        <c:axId val="14802157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -805,7 +805,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="43028982"/>
+        <c:crossAx val="98521956"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="1000"/>
       </c:valAx>
@@ -839,7 +839,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1388,11 +1388,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="45618842"/>
-        <c:axId val="15265379"/>
+        <c:axId val="19254119"/>
+        <c:axId val="93459433"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45618842"/>
+        <c:axId val="19254119"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -1434,12 +1434,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15265379"/>
+        <c:crossAx val="93459433"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15265379"/>
+        <c:axId val="93459433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1479,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45618842"/>
+        <c:crossAx val="19254119"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1512,7 +1512,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2061,11 +2061,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="68831368"/>
-        <c:axId val="2853699"/>
+        <c:axId val="86532144"/>
+        <c:axId val="99439649"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68831368"/>
+        <c:axId val="86532144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -2107,12 +2107,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2853699"/>
+        <c:crossAx val="99439649"/>
         <c:crossesAt val="1"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2853699"/>
+        <c:axId val="99439649"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:logBase val="10"/>
@@ -2154,7 +2154,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68831368"/>
+        <c:crossAx val="86532144"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2187,7 +2187,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2748,11 +2748,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="18884950"/>
-        <c:axId val="82695163"/>
+        <c:axId val="20637546"/>
+        <c:axId val="91978426"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18884950"/>
+        <c:axId val="20637546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -2794,12 +2794,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82695163"/>
+        <c:crossAx val="91978426"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82695163"/>
+        <c:axId val="91978426"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2839,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18884950"/>
+        <c:crossAx val="20637546"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2872,7 +2872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3433,11 +3433,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="9602099"/>
-        <c:axId val="5340297"/>
+        <c:axId val="22485124"/>
+        <c:axId val="80093819"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9602099"/>
+        <c:axId val="22485124"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -3479,12 +3479,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5340297"/>
+        <c:crossAx val="80093819"/>
         <c:crossesAt val="1"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5340297"/>
+        <c:axId val="80093819"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:logBase val="10"/>
@@ -3526,7 +3526,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="9602099"/>
+        <c:crossAx val="22485124"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3559,7 +3559,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3958,11 +3958,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="27113907"/>
-        <c:axId val="21127376"/>
+        <c:axId val="77601058"/>
+        <c:axId val="48472917"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27113907"/>
+        <c:axId val="77601058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4004,12 +4004,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="21127376"/>
+        <c:crossAx val="48472917"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21127376"/>
+        <c:axId val="48472917"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4049,7 +4049,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27113907"/>
+        <c:crossAx val="77601058"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4082,7 +4082,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4547,11 +4547,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82770833"/>
-        <c:axId val="40611921"/>
+        <c:axId val="3223477"/>
+        <c:axId val="20630040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82770833"/>
+        <c:axId val="3223477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4593,12 +4593,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40611921"/>
+        <c:crossAx val="20630040"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40611921"/>
+        <c:axId val="20630040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4638,7 +4638,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82770833"/>
+        <c:crossAx val="3223477"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4671,7 +4671,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5118,11 +5118,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60145155"/>
-        <c:axId val="23400877"/>
+        <c:axId val="95991690"/>
+        <c:axId val="1358672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60145155"/>
+        <c:axId val="95991690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -5164,12 +5164,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23400877"/>
+        <c:crossAx val="1358672"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23400877"/>
+        <c:axId val="1358672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5209,7 +5209,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60145155"/>
+        <c:crossAx val="95991690"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5242,7 +5242,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5773,11 +5773,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="20353503"/>
-        <c:axId val="82476262"/>
+        <c:axId val="88411772"/>
+        <c:axId val="17339410"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20353503"/>
+        <c:axId val="88411772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5811,11 +5811,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82476262"/>
+        <c:crossAx val="17339410"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82476262"/>
+        <c:axId val="17339410"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5849,7 +5849,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20353503"/>
+        <c:crossAx val="88411772"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -6091,7 +6091,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>325800</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6124,13 +6124,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>563040</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>276120</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6154,13 +6154,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>366840</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>79920</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6184,13 +6184,13 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>176400</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>496800</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8284,8 +8284,8 @@
   </sheetPr>
   <dimension ref="A1:K192"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="A24" activeCellId="0" pane="topLeft" sqref="A24"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="R48" activeCellId="0" pane="topLeft" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8619,6 +8619,7 @@
         <v>0.11260135</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="24">
       <c r="A24" s="9" t="s">
         <v>20</v>
@@ -9009,6 +9010,7 @@
         <v>1.1752745</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="47"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="48">
       <c r="A48" s="9" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Fixed bug in Villeneuve experimental data
</commit_message>
<xml_diff>
--- a/experimental_data/dilution_indicator/Dilution_indicator_data.xlsx
+++ b/experimental_data/dilution_indicator/Dilution_indicator_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="488" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="488" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Villeneuve2003" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="32">
   <si>
     <t>Hepatic.Microcirculation.Isolated.Perfused.Human.Liver_[Human]_Villeneuve1996</t>
   </si>
@@ -403,7 +403,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -712,11 +712,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="98521956"/>
-        <c:axId val="14802157"/>
+        <c:axId val="27511208"/>
+        <c:axId val="69270183"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98521956"/>
+        <c:axId val="27511208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -758,12 +758,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14802157"/>
+        <c:crossAx val="69270183"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14802157"/>
+        <c:axId val="69270183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -805,7 +805,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98521956"/>
+        <c:crossAx val="27511208"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="1000"/>
       </c:valAx>
@@ -839,7 +839,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1388,11 +1388,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="19254119"/>
-        <c:axId val="93459433"/>
+        <c:axId val="17375019"/>
+        <c:axId val="60161029"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19254119"/>
+        <c:axId val="17375019"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -1434,12 +1434,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93459433"/>
+        <c:crossAx val="60161029"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93459433"/>
+        <c:axId val="60161029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1479,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19254119"/>
+        <c:crossAx val="17375019"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1512,7 +1512,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2061,11 +2061,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86532144"/>
-        <c:axId val="99439649"/>
+        <c:axId val="7178654"/>
+        <c:axId val="71776083"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86532144"/>
+        <c:axId val="7178654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -2107,12 +2107,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99439649"/>
+        <c:crossAx val="71776083"/>
         <c:crossesAt val="1"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99439649"/>
+        <c:axId val="71776083"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:logBase val="10"/>
@@ -2154,7 +2154,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86532144"/>
+        <c:crossAx val="7178654"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2187,7 +2187,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2748,11 +2748,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="20637546"/>
-        <c:axId val="91978426"/>
+        <c:axId val="45464712"/>
+        <c:axId val="25067557"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20637546"/>
+        <c:axId val="45464712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -2794,12 +2794,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91978426"/>
+        <c:crossAx val="25067557"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91978426"/>
+        <c:axId val="25067557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2839,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20637546"/>
+        <c:crossAx val="45464712"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2872,7 +2872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3433,11 +3433,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="22485124"/>
-        <c:axId val="80093819"/>
+        <c:axId val="93895815"/>
+        <c:axId val="52197125"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22485124"/>
+        <c:axId val="93895815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -3479,12 +3479,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80093819"/>
+        <c:crossAx val="52197125"/>
         <c:crossesAt val="1"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80093819"/>
+        <c:axId val="52197125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:logBase val="10"/>
@@ -3526,7 +3526,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22485124"/>
+        <c:crossAx val="93895815"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3559,7 +3559,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3958,11 +3958,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77601058"/>
-        <c:axId val="48472917"/>
+        <c:axId val="61307851"/>
+        <c:axId val="37514740"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77601058"/>
+        <c:axId val="61307851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4004,12 +4004,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48472917"/>
+        <c:crossAx val="37514740"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48472917"/>
+        <c:axId val="37514740"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4049,7 +4049,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77601058"/>
+        <c:crossAx val="61307851"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4082,7 +4082,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4547,11 +4547,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="3223477"/>
-        <c:axId val="20630040"/>
+        <c:axId val="63896163"/>
+        <c:axId val="85150303"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3223477"/>
+        <c:axId val="63896163"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -4593,12 +4593,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20630040"/>
+        <c:crossAx val="85150303"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20630040"/>
+        <c:axId val="85150303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4638,7 +4638,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3223477"/>
+        <c:crossAx val="63896163"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -4671,7 +4671,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5118,11 +5118,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95991690"/>
-        <c:axId val="1358672"/>
+        <c:axId val="19301772"/>
+        <c:axId val="2209424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95991690"/>
+        <c:axId val="19301772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -5164,12 +5164,12 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1358672"/>
+        <c:crossAx val="2209424"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1358672"/>
+        <c:axId val="2209424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5209,7 +5209,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95991690"/>
+        <c:crossAx val="19301772"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5242,7 +5242,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5295,7 +5295,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -5385,7 +5385,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -5481,7 +5481,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -5577,7 +5577,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -5673,7 +5673,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -5773,11 +5773,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88411772"/>
-        <c:axId val="17339410"/>
+        <c:axId val="65007809"/>
+        <c:axId val="82803479"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88411772"/>
+        <c:axId val="65007809"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5811,11 +5811,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17339410"/>
+        <c:crossAx val="82803479"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17339410"/>
+        <c:axId val="82803479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5849,7 +5849,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88411772"/>
+        <c:crossAx val="65007809"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -5889,15 +5889,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:colOff>265680</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>127440</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5912,8 +5912,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6339600" y="5721840"/>
-          <a:ext cx="3675240" cy="6255720"/>
+          <a:off x="6366600" y="5712840"/>
+          <a:ext cx="3674880" cy="6255360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5928,15 +5928,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>327240</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>565920</xdr:colOff>
+      <xdr:colOff>592560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5944,8 +5944,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6428160" y="347040"/>
-        <a:ext cx="4814640" cy="2337120"/>
+        <a:off x="6455160" y="338040"/>
+        <a:ext cx="4814280" cy="2336760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5958,15 +5958,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>664200</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>293400</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5974,8 +5974,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11341080" y="363240"/>
-        <a:ext cx="4967640" cy="2337480"/>
+        <a:off x="11368080" y="354240"/>
+        <a:ext cx="4967280" cy="2337120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5988,15 +5988,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>324000</xdr:colOff>
+      <xdr:colOff>350640</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6004,8 +6004,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11520360" y="2766960"/>
-        <a:ext cx="4818960" cy="2337480"/>
+        <a:off x="11547360" y="2757960"/>
+        <a:ext cx="4818600" cy="2337120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6018,15 +6018,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>348480</xdr:colOff>
+      <xdr:colOff>375480</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>354960</xdr:colOff>
+      <xdr:colOff>381600</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6034,8 +6034,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10262520" y="5465520"/>
-        <a:ext cx="6870240" cy="3293280"/>
+        <a:off x="10289520" y="5456520"/>
+        <a:ext cx="6869880" cy="3292920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6048,15 +6048,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>345600</xdr:colOff>
+      <xdr:colOff>372600</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>352080</xdr:colOff>
+      <xdr:colOff>378720</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6064,8 +6064,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10259640" y="8799120"/>
-        <a:ext cx="6870240" cy="3293280"/>
+        <a:off x="10286640" y="8790120"/>
+        <a:ext cx="6869880" cy="3292920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6083,15 +6083,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>389520</xdr:colOff>
+      <xdr:colOff>416520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>325800</xdr:colOff>
+      <xdr:colOff>352440</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6106,8 +6106,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5674320" y="330120"/>
-          <a:ext cx="13663800" cy="5988960"/>
+          <a:off x="5701320" y="321120"/>
+          <a:ext cx="13663440" cy="5988600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6122,15 +6122,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>563040</xdr:colOff>
+      <xdr:colOff>590040</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>276120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6138,8 +6138,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5847840" y="6382080"/>
-        <a:ext cx="5814360" cy="2742480"/>
+        <a:off x="5874840" y="6373080"/>
+        <a:ext cx="5814000" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6152,15 +6152,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>366840</xdr:colOff>
+      <xdr:colOff>393840</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>79920</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6168,8 +6168,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11752920" y="6390360"/>
-        <a:ext cx="5814000" cy="2742480"/>
+        <a:off x="11779920" y="6381360"/>
+        <a:ext cx="5813640" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6182,15 +6182,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>176400</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>496800</xdr:colOff>
+      <xdr:colOff>523440</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6198,8 +6198,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17663400" y="6402240"/>
-        <a:ext cx="5658840" cy="2742480"/>
+        <a:off x="17690400" y="6393240"/>
+        <a:ext cx="5658480" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6217,15 +6217,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>336960</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>47520</xdr:colOff>
+      <xdr:colOff>74160</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6240,8 +6240,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8464680" y="632520"/>
-          <a:ext cx="4587480" cy="7403040"/>
+          <a:off x="8491680" y="623520"/>
+          <a:ext cx="4587120" cy="7402680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6256,15 +6256,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>271080</xdr:colOff>
+      <xdr:colOff>298080</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>790920</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4680</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6272,8 +6272,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="271080" y="2304360"/>
-        <a:ext cx="5396400" cy="4374360"/>
+        <a:off x="298080" y="2295360"/>
+        <a:ext cx="5396040" cy="4374000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6293,8 +6293,8 @@
   </sheetPr>
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A35" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="D97" activeCellId="0" pane="topLeft" sqref="D97"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A38" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="A51" activeCellId="0" pane="topLeft" sqref="A51:D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7361,31 +7361,47 @@
         <v>113.97777</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="50"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="51">
+      <c r="A51" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="52">
       <c r="A52" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="53">
-      <c r="A53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>12</v>
+      <c r="A53" s="0" t="n">
+        <v>10.622453</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>99.81956</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="8" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
-        <v>11.485738</v>
+        <v>10.278376</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>101.32352</v>
+        <v>188.21613</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>3</v>
@@ -7397,10 +7413,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
-        <v>12.491186</v>
+        <v>10.369031</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>291.517</v>
+        <v>365.74756</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>3</v>
@@ -7412,10 +7428,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
-        <v>13.014514</v>
+        <v>10.9005995</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>575.06177</v>
+        <v>766.41064</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>3</v>
@@ -7427,10 +7443,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
-        <v>16.15448</v>
+        <v>12.732246</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>1443.7595</v>
+        <v>1705.5992</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>3</v>
@@ -7442,10 +7458,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
-        <v>17.514307</v>
+        <v>14.539169</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>2375.714</v>
+        <v>3166.6785</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>3</v>
@@ -7457,10 +7473,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
-        <v>20.536835</v>
+        <v>16.716955</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2522.3425</v>
+        <v>3794.3345</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>3</v>
@@ -7472,10 +7488,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
-        <v>25.673275</v>
+        <v>20.975687</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2009.4023</v>
+        <v>2679.182</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>3</v>
@@ -7487,10 +7503,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
-        <v>34.606934</v>
+        <v>23.495491</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>901.29517</v>
+        <v>1677.0084</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>3</v>
@@ -7502,10 +7518,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
-        <v>43.55501</v>
+        <v>26.454145</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>449.33353</v>
+        <v>1114.9784</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>3</v>
@@ -7517,10 +7533,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
-        <v>50.368572</v>
+        <v>32.400303</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>256.71063</v>
+        <v>608.88055</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>3</v>
@@ -7532,10 +7548,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
-        <v>56.765945</v>
+        <v>35.79163</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>163.02415</v>
+        <v>410.95032</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>3</v>
@@ -7547,10 +7563,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
-        <v>60.600246</v>
+        <v>41.298935</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>120.45422</v>
+        <v>211.27925</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>3</v>
@@ -7562,10 +7578,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
-        <v>63.155075</v>
+        <v>46.385925</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>97.460915</v>
+        <v>117.15009</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>3</v>
@@ -8020,7 +8036,7 @@
       <c r="C96" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D96" s="8" t="b">
+      <c r="D96" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8050,7 +8066,7 @@
       <c r="C98" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="8" t="b">
+      <c r="D98" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8065,7 +8081,7 @@
       <c r="C99" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D99" s="8" t="b">
+      <c r="D99" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8080,7 +8096,7 @@
       <c r="C100" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D100" s="8" t="b">
+      <c r="D100" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8095,7 +8111,7 @@
       <c r="C101" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D101" s="8" t="b">
+      <c r="D101" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8110,7 +8126,7 @@
       <c r="C102" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D102" s="8" t="b">
+      <c r="D102" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8125,7 +8141,7 @@
       <c r="C103" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D103" s="8" t="b">
+      <c r="D103" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8140,7 +8156,7 @@
       <c r="C104" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D104" s="8" t="b">
+      <c r="D104" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8155,7 +8171,7 @@
       <c r="C105" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D105" s="8" t="b">
+      <c r="D105" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8170,7 +8186,7 @@
       <c r="C106" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D106" s="8" t="b">
+      <c r="D106" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8185,7 +8201,7 @@
       <c r="C107" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D107" s="8" t="b">
+      <c r="D107" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8200,7 +8216,7 @@
       <c r="C108" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D108" s="8" t="b">
+      <c r="D108" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8215,7 +8231,7 @@
       <c r="C109" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="8" t="b">
+      <c r="D109" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8230,7 +8246,7 @@
       <c r="C110" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D110" s="8" t="b">
+      <c r="D110" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8245,7 +8261,7 @@
       <c r="C111" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="8" t="b">
+      <c r="D111" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8260,7 +8276,7 @@
       <c r="C112" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D112" s="8" t="b">
+      <c r="D112" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8284,8 +8300,8 @@
   </sheetPr>
   <dimension ref="A1:K192"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="R48" activeCellId="0" pane="topLeft" sqref="R48"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="R48" activeCellId="1" pane="topLeft" sqref="A51:D66 R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11365,7 +11381,7 @@
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="R4" activeCellId="0" pane="topLeft" sqref="R4"/>
+      <selection activeCell="R4" activeCellId="1" pane="topLeft" sqref="A51:D66 R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>